<commit_message>
update: Add BIND env to GoDockerEnv
</commit_message>
<xml_diff>
--- a/GoDNS/MalfareAuth/AdditionalSection/TestResult.xlsx
+++ b/GoDNS/MalfareAuth/AdditionalSection/TestResult.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>类型</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>WKS</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>---待测试---</t>
@@ -273,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -302,9 +299,6 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -324,7 +318,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -637,14 +631,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="17" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="21.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="28.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -661,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -678,7 +672,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -695,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -710,7 +704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -725,7 +719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -740,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -757,7 +751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -772,7 +766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -787,7 +781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -802,7 +796,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -817,107 +811,105 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="5">
         <v>11</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="21" customFormat="1" s="1">
+      <c r="A13" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A13" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="B13" s="5">
         <v>12</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="21" customFormat="1" s="1">
+      <c r="A14" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A14" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="B14" s="5">
         <v>13</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5">
         <v>14</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A16" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5">
         <v>15</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5">
         <v>16</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" s="5">
         <v>28</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>7</v>
@@ -926,149 +918,149 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="5">
         <v>33</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="5">
         <v>41</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="21" customFormat="1" s="1">
+      <c r="A21" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A21" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="B21" s="5">
         <v>43</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="5">
         <v>46</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="5">
         <v>47</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A24" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="5">
         <v>48</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="5">
         <v>50</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="5">
         <v>51</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="21" customFormat="1" s="1">
       <c r="A27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="21" customFormat="1" s="1">
+      <c r="A28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="1">
-      <c r="A28" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>256</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="16" t="s">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>